<commit_message>
Refactor settings, logging, and Docker build process
Reorganized settings files for clarity and improved maintenance by separating environment-specific configurations. Enhanced logging setup for better debugging and monitoring. Refined Docker build and deployment scripts for a consistent and isolated local development environment. Minor code cleanups and addition of static content fixtures.
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/PV-Test-02.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/PV-Test-02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AB2D3B-C2AD-2B4C-BE7A-AD2EB8A78F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF87865-26EE-8347-A004-B3F8D80526CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>Task Name</t>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[PV-374] Add compress swimlane functionality
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/PV-Test-02.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/PV-Test-02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF87865-26EE-8347-A004-B3F8D80526CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7434846F-1B1C-D84A-981B-9B3FF6ED04D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
-    <t>Unique Sticky ID</t>
-  </si>
-  <si>
     <t>Level #</t>
   </si>
   <si>
@@ -118,7 +115,10 @@
     <t>6</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Task Name</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -567,51 +567,51 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="4">
         <v>44927</v>
@@ -627,16 +627,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="4">
         <v>44928</v>
@@ -652,16 +652,16 @@
     </row>
     <row r="4" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4">
         <v>44928</v>
@@ -677,16 +677,16 @@
     </row>
     <row r="5" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="4">
         <v>44928</v>
@@ -695,7 +695,7 @@
         <v>44939</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
@@ -704,16 +704,16 @@
     </row>
     <row r="6" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="4">
         <v>44942</v>
@@ -722,7 +722,7 @@
         <v>44946</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
@@ -731,16 +731,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4">
         <v>44949</v>
@@ -749,7 +749,7 @@
         <v>44953</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5"/>
@@ -758,16 +758,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4">
         <v>44956</v>
@@ -776,7 +776,7 @@
         <v>44967</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>

</xml_diff>